<commit_message>
made a make file
also need to change NULL back to 0 for simpler coding
</commit_message>
<xml_diff>
--- a/Excel Tables.xlsx
+++ b/Excel Tables.xlsx
@@ -2,19 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan Lau\Documents\Github\Mahjong-Score-Calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C59D59-E4C3-47A2-B9CF-4A7646A10531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C6C30C-8A1D-458A-A89C-EA1DE01C493F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{177A03E6-3AE8-4F17-BF48-221432F79E4F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{177A03E6-3AE8-4F17-BF48-221432F79E4F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Dealer" sheetId="1" r:id="rId1"/>
-    <sheet name="Non Dealer" sheetId="2" r:id="rId2"/>
+    <sheet name="Dealer Table" sheetId="1" r:id="rId1"/>
+    <sheet name="Dealer High Hands" sheetId="4" r:id="rId2"/>
+    <sheet name="Non Dealer Table" sheetId="2" r:id="rId3"/>
+    <sheet name="Non Dealer High Hands" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="65">
   <si>
     <t>Han/Fu</t>
   </si>
@@ -108,12 +110,6 @@
     <t>1800 5300</t>
   </si>
   <si>
-    <t>0 2400</t>
-  </si>
-  <si>
-    <t>0 0</t>
-  </si>
-  <si>
     <t>2000 5800</t>
   </si>
   <si>
@@ -132,18 +128,12 @@
     <t>3600 10600</t>
   </si>
   <si>
-    <t>1300 0</t>
-  </si>
-  <si>
     <t>3900 11600</t>
   </si>
   <si>
     <t>4000 12000</t>
   </si>
   <si>
-    <t>2600 0</t>
-  </si>
-  <si>
     <t>6000 18000</t>
   </si>
   <si>
@@ -183,12 +173,6 @@
     <t>900/1800 3600</t>
   </si>
   <si>
-    <t>400/700 0</t>
-  </si>
-  <si>
-    <t>0 1600</t>
-  </si>
-  <si>
     <t>1000/2000 3900</t>
   </si>
   <si>
@@ -207,18 +191,12 @@
     <t>1800/3600 7100</t>
   </si>
   <si>
-    <t>700/1300 0</t>
-  </si>
-  <si>
     <t>2000/3900 7700</t>
   </si>
   <si>
     <t>2000/4000 8000</t>
   </si>
   <si>
-    <t>1300/2600 0</t>
-  </si>
-  <si>
     <t>3000/6000 12000</t>
   </si>
   <si>
@@ -229,6 +207,33 @@
   </si>
   <si>
     <t>8000/16000 32000</t>
+  </si>
+  <si>
+    <t>NULL NULL</t>
+  </si>
+  <si>
+    <t>700 NULL</t>
+  </si>
+  <si>
+    <t>1300 NULL</t>
+  </si>
+  <si>
+    <t>2600 NULL</t>
+  </si>
+  <si>
+    <t>NULL 2400</t>
+  </si>
+  <si>
+    <t>400/700 NULL</t>
+  </si>
+  <si>
+    <t>700/1300 NULL</t>
+  </si>
+  <si>
+    <t>1300/2600 NULL</t>
+  </si>
+  <si>
+    <t>NULL 1600</t>
   </si>
 </sst>
 </file>
@@ -606,10 +611,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45156CA7-69D6-48A3-924E-A67E7B1E7D5F}">
-  <dimension ref="A1:L18"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A18"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -664,10 +670,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -701,11 +707,11 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>700</v>
+      <c r="B3" t="s">
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
@@ -717,22 +723,22 @@
         <v>21</v>
       </c>
       <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
         <v>25</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>26</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>27</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>28</v>
-      </c>
-      <c r="K3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -740,37 +746,37 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
       </c>
       <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>27</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>29</v>
       </c>
-      <c r="G4" t="s">
-        <v>32</v>
-      </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -778,109 +784,37 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
         <v>29</v>
       </c>
-      <c r="D5" t="s">
-        <v>32</v>
-      </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -890,19 +824,107 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B494FBA-26DB-4F7F-A7C2-8030BBD4F5F2}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E69DE3-79E1-4C9A-90FA-664B29AAAACD}">
-  <dimension ref="A1:L18"/>
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -948,37 +970,37 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" t="s">
         <v>39</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
         <v>40</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>41</v>
       </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
         <v>42</v>
       </c>
-      <c r="H2" t="s">
+      <c r="L2" t="s">
         <v>43</v>
-      </c>
-      <c r="I2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" t="s">
-        <v>45</v>
-      </c>
-      <c r="K2" t="s">
-        <v>46</v>
-      </c>
-      <c r="L2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -986,37 +1008,37 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" t="s">
         <v>48</v>
       </c>
-      <c r="C3" t="s">
+      <c r="L3" t="s">
         <v>49</v>
-      </c>
-      <c r="D3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I3" t="s">
-        <v>52</v>
-      </c>
-      <c r="J3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K3" t="s">
-        <v>54</v>
-      </c>
-      <c r="L3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -1024,37 +1046,37 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
         <v>46</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" t="s">
         <v>50</v>
       </c>
-      <c r="E4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" t="s">
-        <v>57</v>
-      </c>
       <c r="H4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="I4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="J4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="K4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="L4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1062,109 +1084,128 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C950714-96EE-45F6-9E3E-101A1D97543D}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
         <v>54</v>
       </c>
-      <c r="D5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F5" t="s">
-        <v>58</v>
-      </c>
-      <c r="G5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H5" t="s">
-        <v>58</v>
-      </c>
-      <c r="I5" t="s">
-        <v>58</v>
-      </c>
-      <c r="J5" t="s">
-        <v>58</v>
-      </c>
-      <c r="K5" t="s">
-        <v>58</v>
-      </c>
-      <c r="L5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B18" t="s">
-        <v>63</v>
+      <c r="B9" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>